<commit_message>
CHD column excluded, new plots drawn
</commit_message>
<xml_diff>
--- a/binary_heart_data.xlsx
+++ b/binary_heart_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K463"/>
+  <dimension ref="A1:J463"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -412,11 +412,6 @@
           <t>age</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>chd</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -449,9 +444,6 @@
       <c r="J2" t="n">
         <v>52</v>
       </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -483,9 +475,6 @@
       </c>
       <c r="J3" t="n">
         <v>63</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -519,9 +508,6 @@
       <c r="J4" t="n">
         <v>46</v>
       </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -554,9 +540,6 @@
       <c r="J5" t="n">
         <v>58</v>
       </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -589,9 +572,6 @@
       <c r="J6" t="n">
         <v>49</v>
       </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -624,9 +604,6 @@
       <c r="J7" t="n">
         <v>45</v>
       </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -659,9 +636,6 @@
       <c r="J8" t="n">
         <v>38</v>
       </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -694,9 +668,6 @@
       <c r="J9" t="n">
         <v>58</v>
       </c>
-      <c r="K9" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -729,9 +700,6 @@
       <c r="J10" t="n">
         <v>29</v>
       </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -764,9 +732,6 @@
       <c r="J11" t="n">
         <v>53</v>
       </c>
-      <c r="K11" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -799,9 +764,6 @@
       <c r="J12" t="n">
         <v>60</v>
       </c>
-      <c r="K12" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -834,9 +796,6 @@
       <c r="J13" t="n">
         <v>40</v>
       </c>
-      <c r="K13" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -869,9 +828,6 @@
       <c r="J14" t="n">
         <v>17</v>
       </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -904,9 +860,6 @@
       <c r="J15" t="n">
         <v>15</v>
       </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -939,9 +892,6 @@
       <c r="J16" t="n">
         <v>53</v>
       </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -974,9 +924,6 @@
       <c r="J17" t="n">
         <v>46</v>
       </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1009,9 +956,6 @@
       <c r="J18" t="n">
         <v>49</v>
       </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1044,9 +988,6 @@
       <c r="J19" t="n">
         <v>53</v>
       </c>
-      <c r="K19" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1079,9 +1020,6 @@
       <c r="J20" t="n">
         <v>62</v>
       </c>
-      <c r="K20" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1114,9 +1052,6 @@
       <c r="J21" t="n">
         <v>59</v>
       </c>
-      <c r="K21" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1149,9 +1084,6 @@
       <c r="J22" t="n">
         <v>20</v>
       </c>
-      <c r="K22" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1184,9 +1116,6 @@
       <c r="J23" t="n">
         <v>44</v>
       </c>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1219,9 +1148,6 @@
       <c r="J24" t="n">
         <v>50</v>
       </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1254,9 +1180,6 @@
       <c r="J25" t="n">
         <v>58</v>
       </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1289,9 +1212,6 @@
       <c r="J26" t="n">
         <v>50</v>
       </c>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1324,9 +1244,6 @@
       <c r="J27" t="n">
         <v>42</v>
       </c>
-      <c r="K27" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1359,9 +1276,6 @@
       <c r="J28" t="n">
         <v>48</v>
       </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1394,9 +1308,6 @@
       <c r="J29" t="n">
         <v>61</v>
       </c>
-      <c r="K29" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1429,9 +1340,6 @@
       <c r="J30" t="n">
         <v>56</v>
       </c>
-      <c r="K30" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1464,9 +1372,6 @@
       <c r="J31" t="n">
         <v>63</v>
       </c>
-      <c r="K31" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1499,9 +1404,6 @@
       <c r="J32" t="n">
         <v>45</v>
       </c>
-      <c r="K32" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1534,9 +1436,6 @@
       <c r="J33" t="n">
         <v>46</v>
       </c>
-      <c r="K33" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1569,9 +1468,6 @@
       <c r="J34" t="n">
         <v>59</v>
       </c>
-      <c r="K34" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1604,9 +1500,6 @@
       <c r="J35" t="n">
         <v>41</v>
       </c>
-      <c r="K35" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1639,9 +1532,6 @@
       <c r="J36" t="n">
         <v>48</v>
       </c>
-      <c r="K36" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1674,9 +1564,6 @@
       <c r="J37" t="n">
         <v>28</v>
       </c>
-      <c r="K37" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1709,9 +1596,6 @@
       <c r="J38" t="n">
         <v>32</v>
       </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1744,9 +1628,6 @@
       <c r="J39" t="n">
         <v>46</v>
       </c>
-      <c r="K39" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1779,9 +1660,6 @@
       <c r="J40" t="n">
         <v>29</v>
       </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1814,9 +1692,6 @@
       <c r="J41" t="n">
         <v>58</v>
       </c>
-      <c r="K41" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1849,9 +1724,6 @@
       <c r="J42" t="n">
         <v>41</v>
       </c>
-      <c r="K42" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1884,9 +1756,6 @@
       <c r="J43" t="n">
         <v>30</v>
       </c>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1919,9 +1788,6 @@
       <c r="J44" t="n">
         <v>15</v>
       </c>
-      <c r="K44" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1954,9 +1820,6 @@
       <c r="J45" t="n">
         <v>51</v>
       </c>
-      <c r="K45" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1989,9 +1852,6 @@
       <c r="J46" t="n">
         <v>17</v>
       </c>
-      <c r="K46" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2024,9 +1884,6 @@
       <c r="J47" t="n">
         <v>48</v>
       </c>
-      <c r="K47" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2059,9 +1916,6 @@
       <c r="J48" t="n">
         <v>58</v>
       </c>
-      <c r="K48" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2094,9 +1948,6 @@
       <c r="J49" t="n">
         <v>33</v>
       </c>
-      <c r="K49" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2129,9 +1980,6 @@
       <c r="J50" t="n">
         <v>16</v>
       </c>
-      <c r="K50" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2164,9 +2012,6 @@
       <c r="J51" t="n">
         <v>30</v>
       </c>
-      <c r="K51" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2199,9 +2044,6 @@
       <c r="J52" t="n">
         <v>42</v>
       </c>
-      <c r="K52" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2234,9 +2076,6 @@
       <c r="J53" t="n">
         <v>49</v>
       </c>
-      <c r="K53" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2269,9 +2108,6 @@
       <c r="J54" t="n">
         <v>42</v>
       </c>
-      <c r="K54" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2304,9 +2140,6 @@
       <c r="J55" t="n">
         <v>31</v>
       </c>
-      <c r="K55" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2339,9 +2172,6 @@
       <c r="J56" t="n">
         <v>53</v>
       </c>
-      <c r="K56" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2374,9 +2204,6 @@
       <c r="J57" t="n">
         <v>48</v>
       </c>
-      <c r="K57" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2409,9 +2236,6 @@
       <c r="J58" t="n">
         <v>28</v>
       </c>
-      <c r="K58" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2444,9 +2268,6 @@
       <c r="J59" t="n">
         <v>38</v>
       </c>
-      <c r="K59" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2479,9 +2300,6 @@
       <c r="J60" t="n">
         <v>18</v>
       </c>
-      <c r="K60" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2514,9 +2332,6 @@
       <c r="J61" t="n">
         <v>61</v>
       </c>
-      <c r="K61" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2549,9 +2364,6 @@
       <c r="J62" t="n">
         <v>33</v>
       </c>
-      <c r="K62" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2584,9 +2396,6 @@
       <c r="J63" t="n">
         <v>44</v>
       </c>
-      <c r="K63" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2619,9 +2428,6 @@
       <c r="J64" t="n">
         <v>57</v>
       </c>
-      <c r="K64" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2654,9 +2460,6 @@
       <c r="J65" t="n">
         <v>38</v>
       </c>
-      <c r="K65" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2689,9 +2492,6 @@
       <c r="J66" t="n">
         <v>17</v>
       </c>
-      <c r="K66" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2724,9 +2524,6 @@
       <c r="J67" t="n">
         <v>54</v>
       </c>
-      <c r="K67" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2759,9 +2556,6 @@
       <c r="J68" t="n">
         <v>30</v>
       </c>
-      <c r="K68" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2794,9 +2588,6 @@
       <c r="J69" t="n">
         <v>27</v>
       </c>
-      <c r="K69" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2829,9 +2620,6 @@
       <c r="J70" t="n">
         <v>33</v>
       </c>
-      <c r="K70" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2864,9 +2652,6 @@
       <c r="J71" t="n">
         <v>32</v>
       </c>
-      <c r="K71" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2899,9 +2684,6 @@
       <c r="J72" t="n">
         <v>15</v>
       </c>
-      <c r="K72" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2934,9 +2716,6 @@
       <c r="J73" t="n">
         <v>26</v>
       </c>
-      <c r="K73" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2969,9 +2748,6 @@
       <c r="J74" t="n">
         <v>36</v>
       </c>
-      <c r="K74" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -3004,9 +2780,6 @@
       <c r="J75" t="n">
         <v>20</v>
       </c>
-      <c r="K75" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -3039,9 +2812,6 @@
       <c r="J76" t="n">
         <v>34</v>
       </c>
-      <c r="K76" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -3074,9 +2844,6 @@
       <c r="J77" t="n">
         <v>40</v>
       </c>
-      <c r="K77" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -3109,9 +2876,6 @@
       <c r="J78" t="n">
         <v>55</v>
       </c>
-      <c r="K78" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -3144,9 +2908,6 @@
       <c r="J79" t="n">
         <v>55</v>
       </c>
-      <c r="K79" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -3179,9 +2940,6 @@
       <c r="J80" t="n">
         <v>56</v>
       </c>
-      <c r="K80" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -3214,9 +2972,6 @@
       <c r="J81" t="n">
         <v>39</v>
       </c>
-      <c r="K81" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -3249,9 +3004,6 @@
       <c r="J82" t="n">
         <v>45</v>
       </c>
-      <c r="K82" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -3284,9 +3036,6 @@
       <c r="J83" t="n">
         <v>53</v>
       </c>
-      <c r="K83" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -3319,9 +3068,6 @@
       <c r="J84" t="n">
         <v>55</v>
       </c>
-      <c r="K84" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -3354,9 +3100,6 @@
       <c r="J85" t="n">
         <v>57</v>
       </c>
-      <c r="K85" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -3389,9 +3132,6 @@
       <c r="J86" t="n">
         <v>17</v>
       </c>
-      <c r="K86" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -3424,9 +3164,6 @@
       <c r="J87" t="n">
         <v>45</v>
       </c>
-      <c r="K87" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -3459,9 +3196,6 @@
       <c r="J88" t="n">
         <v>49</v>
       </c>
-      <c r="K88" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -3494,9 +3228,6 @@
       <c r="J89" t="n">
         <v>38</v>
       </c>
-      <c r="K89" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -3529,9 +3260,6 @@
       <c r="J90" t="n">
         <v>41</v>
       </c>
-      <c r="K90" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -3564,9 +3292,6 @@
       <c r="J91" t="n">
         <v>55</v>
       </c>
-      <c r="K91" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -3599,9 +3324,6 @@
       <c r="J92" t="n">
         <v>21</v>
       </c>
-      <c r="K92" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -3634,9 +3356,6 @@
       <c r="J93" t="n">
         <v>64</v>
       </c>
-      <c r="K93" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -3669,9 +3388,6 @@
       <c r="J94" t="n">
         <v>29</v>
       </c>
-      <c r="K94" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -3704,9 +3420,6 @@
       <c r="J95" t="n">
         <v>49</v>
       </c>
-      <c r="K95" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -3739,9 +3452,6 @@
       <c r="J96" t="n">
         <v>56</v>
       </c>
-      <c r="K96" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -3774,9 +3484,6 @@
       <c r="J97" t="n">
         <v>62</v>
       </c>
-      <c r="K97" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -3809,9 +3516,6 @@
       <c r="J98" t="n">
         <v>29</v>
       </c>
-      <c r="K98" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -3844,9 +3548,6 @@
       <c r="J99" t="n">
         <v>39</v>
       </c>
-      <c r="K99" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -3879,9 +3580,6 @@
       <c r="J100" t="n">
         <v>51</v>
       </c>
-      <c r="K100" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -3914,9 +3612,6 @@
       <c r="J101" t="n">
         <v>39</v>
       </c>
-      <c r="K101" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -3949,9 +3644,6 @@
       <c r="J102" t="n">
         <v>50</v>
       </c>
-      <c r="K102" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3984,9 +3676,6 @@
       <c r="J103" t="n">
         <v>27</v>
       </c>
-      <c r="K103" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -4019,9 +3708,6 @@
       <c r="J104" t="n">
         <v>46</v>
       </c>
-      <c r="K104" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -4054,9 +3740,6 @@
       <c r="J105" t="n">
         <v>31</v>
       </c>
-      <c r="K105" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -4089,9 +3772,6 @@
       <c r="J106" t="n">
         <v>29</v>
       </c>
-      <c r="K106" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -4124,9 +3804,6 @@
       <c r="J107" t="n">
         <v>64</v>
       </c>
-      <c r="K107" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -4159,9 +3836,6 @@
       <c r="J108" t="n">
         <v>61</v>
       </c>
-      <c r="K108" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -4194,9 +3868,6 @@
       <c r="J109" t="n">
         <v>54</v>
       </c>
-      <c r="K109" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -4229,9 +3900,6 @@
       <c r="J110" t="n">
         <v>42</v>
       </c>
-      <c r="K110" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -4264,9 +3932,6 @@
       <c r="J111" t="n">
         <v>18</v>
       </c>
-      <c r="K111" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -4299,9 +3964,6 @@
       <c r="J112" t="n">
         <v>16</v>
       </c>
-      <c r="K112" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -4334,9 +3996,6 @@
       <c r="J113" t="n">
         <v>54</v>
       </c>
-      <c r="K113" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -4369,9 +4028,6 @@
       <c r="J114" t="n">
         <v>37</v>
       </c>
-      <c r="K114" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -4404,9 +4060,6 @@
       <c r="J115" t="n">
         <v>61</v>
       </c>
-      <c r="K115" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -4439,9 +4092,6 @@
       <c r="J116" t="n">
         <v>59</v>
       </c>
-      <c r="K116" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -4474,9 +4124,6 @@
       <c r="J117" t="n">
         <v>48</v>
       </c>
-      <c r="K117" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -4509,9 +4156,6 @@
       <c r="J118" t="n">
         <v>32</v>
       </c>
-      <c r="K118" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -4544,9 +4188,6 @@
       <c r="J119" t="n">
         <v>42</v>
       </c>
-      <c r="K119" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -4579,9 +4220,6 @@
       <c r="J120" t="n">
         <v>61</v>
       </c>
-      <c r="K120" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -4614,9 +4252,6 @@
       <c r="J121" t="n">
         <v>27</v>
       </c>
-      <c r="K121" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -4649,9 +4284,6 @@
       <c r="J122" t="n">
         <v>60</v>
       </c>
-      <c r="K122" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -4684,9 +4316,6 @@
       <c r="J123" t="n">
         <v>28</v>
       </c>
-      <c r="K123" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -4719,9 +4348,6 @@
       <c r="J124" t="n">
         <v>33</v>
       </c>
-      <c r="K124" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -4754,9 +4380,6 @@
       <c r="J125" t="n">
         <v>56</v>
       </c>
-      <c r="K125" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -4789,9 +4412,6 @@
       <c r="J126" t="n">
         <v>45</v>
       </c>
-      <c r="K126" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -4824,9 +4444,6 @@
       <c r="J127" t="n">
         <v>59</v>
       </c>
-      <c r="K127" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -4859,9 +4476,6 @@
       <c r="J128" t="n">
         <v>28</v>
       </c>
-      <c r="K128" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -4894,9 +4508,6 @@
       <c r="J129" t="n">
         <v>38</v>
       </c>
-      <c r="K129" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -4929,9 +4540,6 @@
       <c r="J130" t="n">
         <v>60</v>
       </c>
-      <c r="K130" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -4964,9 +4572,6 @@
       <c r="J131" t="n">
         <v>64</v>
       </c>
-      <c r="K131" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -4999,9 +4604,6 @@
       <c r="J132" t="n">
         <v>62</v>
       </c>
-      <c r="K132" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -5034,9 +4636,6 @@
       <c r="J133" t="n">
         <v>58</v>
       </c>
-      <c r="K133" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -5069,9 +4668,6 @@
       <c r="J134" t="n">
         <v>30</v>
       </c>
-      <c r="K134" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -5104,9 +4700,6 @@
       <c r="J135" t="n">
         <v>54</v>
       </c>
-      <c r="K135" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -5139,9 +4732,6 @@
       <c r="J136" t="n">
         <v>40</v>
       </c>
-      <c r="K136" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -5174,9 +4764,6 @@
       <c r="J137" t="n">
         <v>52</v>
       </c>
-      <c r="K137" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -5209,9 +4796,6 @@
       <c r="J138" t="n">
         <v>32</v>
       </c>
-      <c r="K138" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -5244,9 +4828,6 @@
       <c r="J139" t="n">
         <v>28</v>
       </c>
-      <c r="K139" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -5279,9 +4860,6 @@
       <c r="J140" t="n">
         <v>20</v>
       </c>
-      <c r="K140" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -5314,9 +4892,6 @@
       <c r="J141" t="n">
         <v>54</v>
       </c>
-      <c r="K141" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -5349,9 +4924,6 @@
       <c r="J142" t="n">
         <v>54</v>
       </c>
-      <c r="K142" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -5384,9 +4956,6 @@
       <c r="J143" t="n">
         <v>25</v>
       </c>
-      <c r="K143" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -5419,9 +4988,6 @@
       <c r="J144" t="n">
         <v>38</v>
       </c>
-      <c r="K144" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -5454,9 +5020,6 @@
       <c r="J145" t="n">
         <v>58</v>
       </c>
-      <c r="K145" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -5489,9 +5052,6 @@
       <c r="J146" t="n">
         <v>40</v>
       </c>
-      <c r="K146" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -5524,9 +5084,6 @@
       <c r="J147" t="n">
         <v>40</v>
       </c>
-      <c r="K147" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -5559,9 +5116,6 @@
       <c r="J148" t="n">
         <v>31</v>
       </c>
-      <c r="K148" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -5594,9 +5148,6 @@
       <c r="J149" t="n">
         <v>43</v>
       </c>
-      <c r="K149" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -5629,9 +5180,6 @@
       <c r="J150" t="n">
         <v>33</v>
       </c>
-      <c r="K150" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -5664,9 +5212,6 @@
       <c r="J151" t="n">
         <v>61</v>
       </c>
-      <c r="K151" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -5699,9 +5244,6 @@
       <c r="J152" t="n">
         <v>55</v>
       </c>
-      <c r="K152" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -5734,9 +5276,6 @@
       <c r="J153" t="n">
         <v>52</v>
       </c>
-      <c r="K153" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -5769,9 +5308,6 @@
       <c r="J154" t="n">
         <v>24</v>
       </c>
-      <c r="K154" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -5804,9 +5340,6 @@
       <c r="J155" t="n">
         <v>20</v>
       </c>
-      <c r="K155" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -5839,9 +5372,6 @@
       <c r="J156" t="n">
         <v>41</v>
       </c>
-      <c r="K156" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -5874,9 +5404,6 @@
       <c r="J157" t="n">
         <v>55</v>
       </c>
-      <c r="K157" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -5909,9 +5436,6 @@
       <c r="J158" t="n">
         <v>17</v>
       </c>
-      <c r="K158" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -5944,9 +5468,6 @@
       <c r="J159" t="n">
         <v>53</v>
       </c>
-      <c r="K159" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -5979,9 +5500,6 @@
       <c r="J160" t="n">
         <v>38</v>
       </c>
-      <c r="K160" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -6014,9 +5532,6 @@
       <c r="J161" t="n">
         <v>43</v>
       </c>
-      <c r="K161" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -6049,9 +5564,6 @@
       <c r="J162" t="n">
         <v>31</v>
       </c>
-      <c r="K162" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -6084,9 +5596,6 @@
       <c r="J163" t="n">
         <v>62</v>
       </c>
-      <c r="K163" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -6119,9 +5628,6 @@
       <c r="J164" t="n">
         <v>16</v>
       </c>
-      <c r="K164" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -6154,9 +5660,6 @@
       <c r="J165" t="n">
         <v>21</v>
       </c>
-      <c r="K165" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -6189,9 +5692,6 @@
       <c r="J166" t="n">
         <v>16</v>
       </c>
-      <c r="K166" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -6224,9 +5724,6 @@
       <c r="J167" t="n">
         <v>49</v>
       </c>
-      <c r="K167" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -6259,9 +5756,6 @@
       <c r="J168" t="n">
         <v>55</v>
       </c>
-      <c r="K168" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -6294,9 +5788,6 @@
       <c r="J169" t="n">
         <v>43</v>
       </c>
-      <c r="K169" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -6329,9 +5820,6 @@
       <c r="J170" t="n">
         <v>25</v>
       </c>
-      <c r="K170" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -6364,9 +5852,6 @@
       <c r="J171" t="n">
         <v>48</v>
       </c>
-      <c r="K171" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -6399,9 +5884,6 @@
       <c r="J172" t="n">
         <v>41</v>
       </c>
-      <c r="K172" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -6434,9 +5916,6 @@
       <c r="J173" t="n">
         <v>32</v>
       </c>
-      <c r="K173" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -6469,9 +5948,6 @@
       <c r="J174" t="n">
         <v>47</v>
       </c>
-      <c r="K174" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -6504,9 +5980,6 @@
       <c r="J175" t="n">
         <v>61</v>
       </c>
-      <c r="K175" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -6539,9 +6012,6 @@
       <c r="J176" t="n">
         <v>62</v>
       </c>
-      <c r="K176" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -6574,9 +6044,6 @@
       <c r="J177" t="n">
         <v>61</v>
       </c>
-      <c r="K177" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -6609,9 +6076,6 @@
       <c r="J178" t="n">
         <v>37</v>
       </c>
-      <c r="K178" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -6644,9 +6108,6 @@
       <c r="J179" t="n">
         <v>17</v>
       </c>
-      <c r="K179" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -6679,9 +6140,6 @@
       <c r="J180" t="n">
         <v>24</v>
       </c>
-      <c r="K180" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -6714,9 +6172,6 @@
       <c r="J181" t="n">
         <v>56</v>
       </c>
-      <c r="K181" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -6749,9 +6204,6 @@
       <c r="J182" t="n">
         <v>56</v>
       </c>
-      <c r="K182" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -6784,9 +6236,6 @@
       <c r="J183" t="n">
         <v>51</v>
       </c>
-      <c r="K183" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -6819,9 +6268,6 @@
       <c r="J184" t="n">
         <v>60</v>
       </c>
-      <c r="K184" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -6854,9 +6300,6 @@
       <c r="J185" t="n">
         <v>39</v>
       </c>
-      <c r="K185" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -6889,9 +6332,6 @@
       <c r="J186" t="n">
         <v>48</v>
       </c>
-      <c r="K186" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -6924,9 +6364,6 @@
       <c r="J187" t="n">
         <v>33</v>
       </c>
-      <c r="K187" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -6959,9 +6396,6 @@
       <c r="J188" t="n">
         <v>63</v>
       </c>
-      <c r="K188" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -6994,9 +6428,6 @@
       <c r="J189" t="n">
         <v>39</v>
       </c>
-      <c r="K189" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -7029,9 +6460,6 @@
       <c r="J190" t="n">
         <v>63</v>
       </c>
-      <c r="K190" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -7064,9 +6492,6 @@
       <c r="J191" t="n">
         <v>64</v>
       </c>
-      <c r="K191" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -7099,9 +6524,6 @@
       <c r="J192" t="n">
         <v>40</v>
       </c>
-      <c r="K192" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -7134,9 +6556,6 @@
       <c r="J193" t="n">
         <v>49</v>
       </c>
-      <c r="K193" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -7169,9 +6588,6 @@
       <c r="J194" t="n">
         <v>39</v>
       </c>
-      <c r="K194" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -7204,9 +6620,6 @@
       <c r="J195" t="n">
         <v>23</v>
       </c>
-      <c r="K195" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -7239,9 +6652,6 @@
       <c r="J196" t="n">
         <v>18</v>
       </c>
-      <c r="K196" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -7274,9 +6684,6 @@
       <c r="J197" t="n">
         <v>21</v>
       </c>
-      <c r="K197" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -7309,9 +6716,6 @@
       <c r="J198" t="n">
         <v>17</v>
       </c>
-      <c r="K198" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -7344,9 +6748,6 @@
       <c r="J199" t="n">
         <v>42</v>
       </c>
-      <c r="K199" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -7379,9 +6780,6 @@
       <c r="J200" t="n">
         <v>54</v>
       </c>
-      <c r="K200" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -7414,9 +6812,6 @@
       <c r="J201" t="n">
         <v>27</v>
       </c>
-      <c r="K201" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -7449,9 +6844,6 @@
       <c r="J202" t="n">
         <v>23</v>
       </c>
-      <c r="K202" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -7484,9 +6876,6 @@
       <c r="J203" t="n">
         <v>31</v>
       </c>
-      <c r="K203" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -7519,9 +6908,6 @@
       <c r="J204" t="n">
         <v>33</v>
       </c>
-      <c r="K204" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -7554,9 +6940,6 @@
       <c r="J205" t="n">
         <v>64</v>
       </c>
-      <c r="K205" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -7589,9 +6972,6 @@
       <c r="J206" t="n">
         <v>58</v>
       </c>
-      <c r="K206" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -7624,9 +7004,6 @@
       <c r="J207" t="n">
         <v>40</v>
       </c>
-      <c r="K207" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -7659,9 +7036,6 @@
       <c r="J208" t="n">
         <v>18</v>
       </c>
-      <c r="K208" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -7694,9 +7068,6 @@
       <c r="J209" t="n">
         <v>60</v>
       </c>
-      <c r="K209" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -7729,9 +7100,6 @@
       <c r="J210" t="n">
         <v>59</v>
       </c>
-      <c r="K210" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -7764,9 +7132,6 @@
       <c r="J211" t="n">
         <v>60</v>
       </c>
-      <c r="K211" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -7799,9 +7164,6 @@
       <c r="J212" t="n">
         <v>60</v>
       </c>
-      <c r="K212" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -7834,9 +7196,6 @@
       <c r="J213" t="n">
         <v>40</v>
       </c>
-      <c r="K213" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -7869,9 +7228,6 @@
       <c r="J214" t="n">
         <v>44</v>
       </c>
-      <c r="K214" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -7904,9 +7260,6 @@
       <c r="J215" t="n">
         <v>53</v>
       </c>
-      <c r="K215" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -7939,9 +7292,6 @@
       <c r="J216" t="n">
         <v>18</v>
       </c>
-      <c r="K216" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -7974,9 +7324,6 @@
       <c r="J217" t="n">
         <v>62</v>
       </c>
-      <c r="K217" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -8009,9 +7356,6 @@
       <c r="J218" t="n">
         <v>45</v>
       </c>
-      <c r="K218" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -8044,9 +7388,6 @@
       <c r="J219" t="n">
         <v>26</v>
       </c>
-      <c r="K219" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -8079,9 +7420,6 @@
       <c r="J220" t="n">
         <v>25</v>
       </c>
-      <c r="K220" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -8114,9 +7452,6 @@
       <c r="J221" t="n">
         <v>57</v>
       </c>
-      <c r="K221" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -8149,9 +7484,6 @@
       <c r="J222" t="n">
         <v>16</v>
       </c>
-      <c r="K222" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -8184,9 +7516,6 @@
       <c r="J223" t="n">
         <v>46</v>
       </c>
-      <c r="K223" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -8219,9 +7548,6 @@
       <c r="J224" t="n">
         <v>60</v>
       </c>
-      <c r="K224" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -8254,9 +7580,6 @@
       <c r="J225" t="n">
         <v>45</v>
       </c>
-      <c r="K225" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -8289,9 +7612,6 @@
       <c r="J226" t="n">
         <v>56</v>
       </c>
-      <c r="K226" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -8324,9 +7644,6 @@
       <c r="J227" t="n">
         <v>42</v>
       </c>
-      <c r="K227" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -8359,9 +7676,6 @@
       <c r="J228" t="n">
         <v>32</v>
       </c>
-      <c r="K228" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -8394,9 +7708,6 @@
       <c r="J229" t="n">
         <v>52</v>
       </c>
-      <c r="K229" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -8429,9 +7740,6 @@
       <c r="J230" t="n">
         <v>64</v>
       </c>
-      <c r="K230" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -8464,9 +7772,6 @@
       <c r="J231" t="n">
         <v>50</v>
       </c>
-      <c r="K231" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -8499,9 +7804,6 @@
       <c r="J232" t="n">
         <v>58</v>
       </c>
-      <c r="K232" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -8534,9 +7836,6 @@
       <c r="J233" t="n">
         <v>62</v>
       </c>
-      <c r="K233" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -8569,9 +7868,6 @@
       <c r="J234" t="n">
         <v>58</v>
       </c>
-      <c r="K234" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -8604,9 +7900,6 @@
       <c r="J235" t="n">
         <v>30</v>
       </c>
-      <c r="K235" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -8639,9 +7932,6 @@
       <c r="J236" t="n">
         <v>29</v>
       </c>
-      <c r="K236" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -8674,9 +7964,6 @@
       <c r="J237" t="n">
         <v>51</v>
       </c>
-      <c r="K237" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -8709,9 +7996,6 @@
       <c r="J238" t="n">
         <v>61</v>
       </c>
-      <c r="K238" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -8744,9 +8028,6 @@
       <c r="J239" t="n">
         <v>57</v>
       </c>
-      <c r="K239" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -8779,9 +8060,6 @@
       <c r="J240" t="n">
         <v>27</v>
       </c>
-      <c r="K240" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -8814,9 +8092,6 @@
       <c r="J241" t="n">
         <v>16</v>
       </c>
-      <c r="K241" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -8849,9 +8124,6 @@
       <c r="J242" t="n">
         <v>45</v>
       </c>
-      <c r="K242" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -8884,9 +8156,6 @@
       <c r="J243" t="n">
         <v>47</v>
       </c>
-      <c r="K243" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -8919,9 +8188,6 @@
       <c r="J244" t="n">
         <v>41</v>
       </c>
-      <c r="K244" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -8954,9 +8220,6 @@
       <c r="J245" t="n">
         <v>55</v>
       </c>
-      <c r="K245" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -8989,9 +8252,6 @@
       <c r="J246" t="n">
         <v>60</v>
       </c>
-      <c r="K246" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -9024,9 +8284,6 @@
       <c r="J247" t="n">
         <v>57</v>
       </c>
-      <c r="K247" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -9059,9 +8316,6 @@
       <c r="J248" t="n">
         <v>56</v>
       </c>
-      <c r="K248" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -9094,9 +8348,6 @@
       <c r="J249" t="n">
         <v>60</v>
       </c>
-      <c r="K249" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -9129,9 +8380,6 @@
       <c r="J250" t="n">
         <v>64</v>
       </c>
-      <c r="K250" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -9164,9 +8412,6 @@
       <c r="J251" t="n">
         <v>58</v>
       </c>
-      <c r="K251" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -9199,9 +8444,6 @@
       <c r="J252" t="n">
         <v>48</v>
       </c>
-      <c r="K252" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -9234,9 +8476,6 @@
       <c r="J253" t="n">
         <v>17</v>
       </c>
-      <c r="K253" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -9269,9 +8508,6 @@
       <c r="J254" t="n">
         <v>63</v>
       </c>
-      <c r="K254" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -9304,9 +8540,6 @@
       <c r="J255" t="n">
         <v>42</v>
       </c>
-      <c r="K255" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -9339,9 +8572,6 @@
       <c r="J256" t="n">
         <v>46</v>
       </c>
-      <c r="K256" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -9374,9 +8604,6 @@
       <c r="J257" t="n">
         <v>54</v>
       </c>
-      <c r="K257" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -9409,9 +8636,6 @@
       <c r="J258" t="n">
         <v>37</v>
       </c>
-      <c r="K258" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -9444,9 +8668,6 @@
       <c r="J259" t="n">
         <v>49</v>
       </c>
-      <c r="K259" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -9479,9 +8700,6 @@
       <c r="J260" t="n">
         <v>58</v>
       </c>
-      <c r="K260" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -9514,9 +8732,6 @@
       <c r="J261" t="n">
         <v>44</v>
       </c>
-      <c r="K261" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -9549,9 +8764,6 @@
       <c r="J262" t="n">
         <v>17</v>
       </c>
-      <c r="K262" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -9584,9 +8796,6 @@
       <c r="J263" t="n">
         <v>20</v>
       </c>
-      <c r="K263" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -9619,9 +8828,6 @@
       <c r="J264" t="n">
         <v>61</v>
       </c>
-      <c r="K264" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -9654,9 +8860,6 @@
       <c r="J265" t="n">
         <v>35</v>
       </c>
-      <c r="K265" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -9689,9 +8892,6 @@
       <c r="J266" t="n">
         <v>52</v>
       </c>
-      <c r="K266" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -9724,9 +8924,6 @@
       <c r="J267" t="n">
         <v>18</v>
       </c>
-      <c r="K267" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -9759,9 +8956,6 @@
       <c r="J268" t="n">
         <v>17</v>
       </c>
-      <c r="K268" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -9794,9 +8988,6 @@
       <c r="J269" t="n">
         <v>57</v>
       </c>
-      <c r="K269" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -9829,9 +9020,6 @@
       <c r="J270" t="n">
         <v>16</v>
       </c>
-      <c r="K270" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -9864,9 +9052,6 @@
       <c r="J271" t="n">
         <v>45</v>
       </c>
-      <c r="K271" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -9899,9 +9084,6 @@
       <c r="J272" t="n">
         <v>55</v>
       </c>
-      <c r="K272" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -9934,9 +9116,6 @@
       <c r="J273" t="n">
         <v>41</v>
       </c>
-      <c r="K273" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -9969,9 +9148,6 @@
       <c r="J274" t="n">
         <v>24</v>
       </c>
-      <c r="K274" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -10004,9 +9180,6 @@
       <c r="J275" t="n">
         <v>43</v>
       </c>
-      <c r="K275" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -10039,9 +9212,6 @@
       <c r="J276" t="n">
         <v>55</v>
       </c>
-      <c r="K276" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -10074,9 +9244,6 @@
       <c r="J277" t="n">
         <v>63</v>
       </c>
-      <c r="K277" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -10109,9 +9276,6 @@
       <c r="J278" t="n">
         <v>64</v>
       </c>
-      <c r="K278" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -10144,9 +9308,6 @@
       <c r="J279" t="n">
         <v>43</v>
       </c>
-      <c r="K279" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -10179,9 +9340,6 @@
       <c r="J280" t="n">
         <v>16</v>
       </c>
-      <c r="K280" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -10214,9 +9372,6 @@
       <c r="J281" t="n">
         <v>16</v>
       </c>
-      <c r="K281" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -10249,9 +9404,6 @@
       <c r="J282" t="n">
         <v>28</v>
       </c>
-      <c r="K282" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -10284,9 +9436,6 @@
       <c r="J283" t="n">
         <v>42</v>
       </c>
-      <c r="K283" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -10319,9 +9468,6 @@
       <c r="J284" t="n">
         <v>50</v>
       </c>
-      <c r="K284" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -10354,9 +9500,6 @@
       <c r="J285" t="n">
         <v>27</v>
       </c>
-      <c r="K285" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -10389,9 +9532,6 @@
       <c r="J286" t="n">
         <v>41</v>
       </c>
-      <c r="K286" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -10424,9 +9564,6 @@
       <c r="J287" t="n">
         <v>17</v>
       </c>
-      <c r="K287" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -10459,9 +9596,6 @@
       <c r="J288" t="n">
         <v>19</v>
       </c>
-      <c r="K288" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -10494,9 +9628,6 @@
       <c r="J289" t="n">
         <v>17</v>
       </c>
-      <c r="K289" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -10529,9 +9660,6 @@
       <c r="J290" t="n">
         <v>16</v>
       </c>
-      <c r="K290" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -10564,9 +9692,6 @@
       <c r="J291" t="n">
         <v>38</v>
       </c>
-      <c r="K291" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -10599,9 +9724,6 @@
       <c r="J292" t="n">
         <v>16</v>
       </c>
-      <c r="K292" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -10634,9 +9756,6 @@
       <c r="J293" t="n">
         <v>16</v>
       </c>
-      <c r="K293" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -10669,9 +9788,6 @@
       <c r="J294" t="n">
         <v>44</v>
       </c>
-      <c r="K294" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -10704,9 +9820,6 @@
       <c r="J295" t="n">
         <v>56</v>
       </c>
-      <c r="K295" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -10739,9 +9852,6 @@
       <c r="J296" t="n">
         <v>34</v>
       </c>
-      <c r="K296" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -10774,9 +9884,6 @@
       <c r="J297" t="n">
         <v>42</v>
       </c>
-      <c r="K297" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -10809,9 +9916,6 @@
       <c r="J298" t="n">
         <v>17</v>
       </c>
-      <c r="K298" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -10844,9 +9948,6 @@
       <c r="J299" t="n">
         <v>17</v>
       </c>
-      <c r="K299" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -10879,9 +9980,6 @@
       <c r="J300" t="n">
         <v>46</v>
       </c>
-      <c r="K300" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -10914,9 +10012,6 @@
       <c r="J301" t="n">
         <v>53</v>
       </c>
-      <c r="K301" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -10949,9 +10044,6 @@
       <c r="J302" t="n">
         <v>45</v>
       </c>
-      <c r="K302" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -10984,9 +10076,6 @@
       <c r="J303" t="n">
         <v>32</v>
       </c>
-      <c r="K303" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -11019,9 +10108,6 @@
       <c r="J304" t="n">
         <v>53</v>
       </c>
-      <c r="K304" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
@@ -11054,9 +10140,6 @@
       <c r="J305" t="n">
         <v>59</v>
       </c>
-      <c r="K305" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -11089,9 +10172,6 @@
       <c r="J306" t="n">
         <v>27</v>
       </c>
-      <c r="K306" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
@@ -11124,9 +10204,6 @@
       <c r="J307" t="n">
         <v>49</v>
       </c>
-      <c r="K307" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -11159,9 +10236,6 @@
       <c r="J308" t="n">
         <v>45</v>
       </c>
-      <c r="K308" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -11194,9 +10268,6 @@
       <c r="J309" t="n">
         <v>59</v>
       </c>
-      <c r="K309" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -11229,9 +10300,6 @@
       <c r="J310" t="n">
         <v>37</v>
       </c>
-      <c r="K310" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -11264,9 +10332,6 @@
       <c r="J311" t="n">
         <v>34</v>
       </c>
-      <c r="K311" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
@@ -11299,9 +10364,6 @@
       <c r="J312" t="n">
         <v>59</v>
       </c>
-      <c r="K312" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
@@ -11334,9 +10396,6 @@
       <c r="J313" t="n">
         <v>46</v>
       </c>
-      <c r="K313" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -11369,9 +10428,6 @@
       <c r="J314" t="n">
         <v>59</v>
       </c>
-      <c r="K314" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
@@ -11404,9 +10460,6 @@
       <c r="J315" t="n">
         <v>44</v>
       </c>
-      <c r="K315" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
@@ -11439,9 +10492,6 @@
       <c r="J316" t="n">
         <v>50</v>
       </c>
-      <c r="K316" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
@@ -11474,9 +10524,6 @@
       <c r="J317" t="n">
         <v>59</v>
       </c>
-      <c r="K317" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -11509,9 +10556,6 @@
       <c r="J318" t="n">
         <v>38</v>
       </c>
-      <c r="K318" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -11544,9 +10588,6 @@
       <c r="J319" t="n">
         <v>26</v>
       </c>
-      <c r="K319" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -11579,9 +10620,6 @@
       <c r="J320" t="n">
         <v>59</v>
       </c>
-      <c r="K320" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -11614,9 +10652,6 @@
       <c r="J321" t="n">
         <v>51</v>
       </c>
-      <c r="K321" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
@@ -11649,9 +10684,6 @@
       <c r="J322" t="n">
         <v>59</v>
       </c>
-      <c r="K322" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
@@ -11684,9 +10716,6 @@
       <c r="J323" t="n">
         <v>38</v>
       </c>
-      <c r="K323" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
@@ -11719,9 +10748,6 @@
       <c r="J324" t="n">
         <v>61</v>
       </c>
-      <c r="K324" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
@@ -11754,9 +10780,6 @@
       <c r="J325" t="n">
         <v>64</v>
       </c>
-      <c r="K325" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
@@ -11789,9 +10812,6 @@
       <c r="J326" t="n">
         <v>55</v>
       </c>
-      <c r="K326" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
@@ -11824,9 +10844,6 @@
       <c r="J327" t="n">
         <v>36</v>
       </c>
-      <c r="K327" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
@@ -11859,9 +10876,6 @@
       <c r="J328" t="n">
         <v>62</v>
       </c>
-      <c r="K328" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -11894,9 +10908,6 @@
       <c r="J329" t="n">
         <v>19</v>
       </c>
-      <c r="K329" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
@@ -11929,9 +10940,6 @@
       <c r="J330" t="n">
         <v>39</v>
       </c>
-      <c r="K330" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -11964,9 +10972,6 @@
       <c r="J331" t="n">
         <v>55</v>
       </c>
-      <c r="K331" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
@@ -11999,9 +11004,6 @@
       <c r="J332" t="n">
         <v>17</v>
       </c>
-      <c r="K332" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
@@ -12034,9 +11036,6 @@
       <c r="J333" t="n">
         <v>45</v>
       </c>
-      <c r="K333" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -12069,9 +11068,6 @@
       <c r="J334" t="n">
         <v>51</v>
       </c>
-      <c r="K334" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
@@ -12104,9 +11100,6 @@
       <c r="J335" t="n">
         <v>59</v>
       </c>
-      <c r="K335" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -12139,9 +11132,6 @@
       <c r="J336" t="n">
         <v>59</v>
       </c>
-      <c r="K336" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -12174,9 +11164,6 @@
       <c r="J337" t="n">
         <v>43</v>
       </c>
-      <c r="K337" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -12209,9 +11196,6 @@
       <c r="J338" t="n">
         <v>58</v>
       </c>
-      <c r="K338" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
@@ -12244,9 +11228,6 @@
       <c r="J339" t="n">
         <v>59</v>
       </c>
-      <c r="K339" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -12279,9 +11260,6 @@
       <c r="J340" t="n">
         <v>27</v>
       </c>
-      <c r="K340" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
@@ -12314,9 +11292,6 @@
       <c r="J341" t="n">
         <v>30</v>
       </c>
-      <c r="K341" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -12349,9 +11324,6 @@
       <c r="J342" t="n">
         <v>40</v>
       </c>
-      <c r="K342" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
@@ -12384,9 +11356,6 @@
       <c r="J343" t="n">
         <v>52</v>
       </c>
-      <c r="K343" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
@@ -12419,9 +11388,6 @@
       <c r="J344" t="n">
         <v>53</v>
       </c>
-      <c r="K344" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
@@ -12454,9 +11420,6 @@
       <c r="J345" t="n">
         <v>31</v>
       </c>
-      <c r="K345" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
@@ -12489,9 +11452,6 @@
       <c r="J346" t="n">
         <v>37</v>
       </c>
-      <c r="K346" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
@@ -12524,9 +11484,6 @@
       <c r="J347" t="n">
         <v>26</v>
       </c>
-      <c r="K347" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
@@ -12559,9 +11516,6 @@
       <c r="J348" t="n">
         <v>53</v>
       </c>
-      <c r="K348" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
@@ -12594,9 +11548,6 @@
       <c r="J349" t="n">
         <v>61</v>
       </c>
-      <c r="K349" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
@@ -12629,9 +11580,6 @@
       <c r="J350" t="n">
         <v>43</v>
       </c>
-      <c r="K350" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
@@ -12664,9 +11612,6 @@
       <c r="J351" t="n">
         <v>60</v>
       </c>
-      <c r="K351" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
@@ -12699,9 +11644,6 @@
       <c r="J352" t="n">
         <v>49</v>
       </c>
-      <c r="K352" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
@@ -12734,9 +11676,6 @@
       <c r="J353" t="n">
         <v>36</v>
       </c>
-      <c r="K353" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
@@ -12769,9 +11708,6 @@
       <c r="J354" t="n">
         <v>58</v>
       </c>
-      <c r="K354" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
@@ -12804,9 +11740,6 @@
       <c r="J355" t="n">
         <v>61</v>
       </c>
-      <c r="K355" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
@@ -12839,9 +11772,6 @@
       <c r="J356" t="n">
         <v>54</v>
       </c>
-      <c r="K356" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
@@ -12874,9 +11804,6 @@
       <c r="J357" t="n">
         <v>58</v>
       </c>
-      <c r="K357" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
@@ -12909,9 +11836,6 @@
       <c r="J358" t="n">
         <v>24</v>
       </c>
-      <c r="K358" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
@@ -12944,9 +11868,6 @@
       <c r="J359" t="n">
         <v>49</v>
       </c>
-      <c r="K359" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
@@ -12979,9 +11900,6 @@
       <c r="J360" t="n">
         <v>50</v>
       </c>
-      <c r="K360" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
@@ -13014,9 +11932,6 @@
       <c r="J361" t="n">
         <v>32</v>
       </c>
-      <c r="K361" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
@@ -13049,9 +11964,6 @@
       <c r="J362" t="n">
         <v>62</v>
       </c>
-      <c r="K362" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
@@ -13084,9 +11996,6 @@
       <c r="J363" t="n">
         <v>34</v>
       </c>
-      <c r="K363" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
@@ -13119,9 +12028,6 @@
       <c r="J364" t="n">
         <v>48</v>
       </c>
-      <c r="K364" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
@@ -13154,9 +12060,6 @@
       <c r="J365" t="n">
         <v>60</v>
       </c>
-      <c r="K365" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
@@ -13189,9 +12092,6 @@
       <c r="J366" t="n">
         <v>52</v>
       </c>
-      <c r="K366" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
@@ -13224,9 +12124,6 @@
       <c r="J367" t="n">
         <v>28</v>
       </c>
-      <c r="K367" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
@@ -13259,9 +12156,6 @@
       <c r="J368" t="n">
         <v>24</v>
       </c>
-      <c r="K368" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
@@ -13294,9 +12188,6 @@
       <c r="J369" t="n">
         <v>30</v>
       </c>
-      <c r="K369" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
@@ -13329,9 +12220,6 @@
       <c r="J370" t="n">
         <v>38</v>
       </c>
-      <c r="K370" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
@@ -13364,9 +12252,6 @@
       <c r="J371" t="n">
         <v>42</v>
       </c>
-      <c r="K371" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
@@ -13399,9 +12284,6 @@
       <c r="J372" t="n">
         <v>64</v>
       </c>
-      <c r="K372" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
@@ -13434,9 +12316,6 @@
       <c r="J373" t="n">
         <v>41</v>
       </c>
-      <c r="K373" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
@@ -13469,9 +12348,6 @@
       <c r="J374" t="n">
         <v>32</v>
       </c>
-      <c r="K374" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
@@ -13504,9 +12380,6 @@
       <c r="J375" t="n">
         <v>64</v>
       </c>
-      <c r="K375" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
@@ -13539,9 +12412,6 @@
       <c r="J376" t="n">
         <v>29</v>
       </c>
-      <c r="K376" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
@@ -13574,9 +12444,6 @@
       <c r="J377" t="n">
         <v>45</v>
       </c>
-      <c r="K377" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
@@ -13609,9 +12476,6 @@
       <c r="J378" t="n">
         <v>31</v>
       </c>
-      <c r="K378" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
@@ -13644,9 +12508,6 @@
       <c r="J379" t="n">
         <v>53</v>
       </c>
-      <c r="K379" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
@@ -13679,9 +12540,6 @@
       <c r="J380" t="n">
         <v>38</v>
       </c>
-      <c r="K380" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
@@ -13714,9 +12572,6 @@
       <c r="J381" t="n">
         <v>64</v>
       </c>
-      <c r="K381" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
@@ -13749,9 +12604,6 @@
       <c r="J382" t="n">
         <v>52</v>
       </c>
-      <c r="K382" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="383">
       <c r="A383" s="1" t="n">
@@ -13784,9 +12636,6 @@
       <c r="J383" t="n">
         <v>44</v>
       </c>
-      <c r="K383" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
@@ -13819,9 +12668,6 @@
       <c r="J384" t="n">
         <v>38</v>
       </c>
-      <c r="K384" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="385">
       <c r="A385" s="1" t="n">
@@ -13854,9 +12700,6 @@
       <c r="J385" t="n">
         <v>31</v>
       </c>
-      <c r="K385" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="386">
       <c r="A386" s="1" t="n">
@@ -13889,9 +12732,6 @@
       <c r="J386" t="n">
         <v>44</v>
       </c>
-      <c r="K386" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="387">
       <c r="A387" s="1" t="n">
@@ -13924,9 +12764,6 @@
       <c r="J387" t="n">
         <v>54</v>
       </c>
-      <c r="K387" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="388">
       <c r="A388" s="1" t="n">
@@ -13959,9 +12796,6 @@
       <c r="J388" t="n">
         <v>59</v>
       </c>
-      <c r="K388" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="389">
       <c r="A389" s="1" t="n">
@@ -13994,9 +12828,6 @@
       <c r="J389" t="n">
         <v>53</v>
       </c>
-      <c r="K389" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="390">
       <c r="A390" s="1" t="n">
@@ -14029,9 +12860,6 @@
       <c r="J390" t="n">
         <v>26</v>
       </c>
-      <c r="K390" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="391">
       <c r="A391" s="1" t="n">
@@ -14064,9 +12892,6 @@
       <c r="J391" t="n">
         <v>53</v>
       </c>
-      <c r="K391" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="392">
       <c r="A392" s="1" t="n">
@@ -14099,9 +12924,6 @@
       <c r="J392" t="n">
         <v>39</v>
       </c>
-      <c r="K392" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="393">
       <c r="A393" s="1" t="n">
@@ -14134,9 +12956,6 @@
       <c r="J393" t="n">
         <v>50</v>
       </c>
-      <c r="K393" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="394">
       <c r="A394" s="1" t="n">
@@ -14169,9 +12988,6 @@
       <c r="J394" t="n">
         <v>61</v>
       </c>
-      <c r="K394" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="395">
       <c r="A395" s="1" t="n">
@@ -14204,9 +13020,6 @@
       <c r="J395" t="n">
         <v>64</v>
       </c>
-      <c r="K395" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="396">
       <c r="A396" s="1" t="n">
@@ -14239,9 +13052,6 @@
       <c r="J396" t="n">
         <v>48</v>
       </c>
-      <c r="K396" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="397">
       <c r="A397" s="1" t="n">
@@ -14274,9 +13084,6 @@
       <c r="J397" t="n">
         <v>27</v>
       </c>
-      <c r="K397" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="398">
       <c r="A398" s="1" t="n">
@@ -14309,9 +13116,6 @@
       <c r="J398" t="n">
         <v>62</v>
       </c>
-      <c r="K398" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="399">
       <c r="A399" s="1" t="n">
@@ -14344,9 +13148,6 @@
       <c r="J399" t="n">
         <v>48</v>
       </c>
-      <c r="K399" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="400">
       <c r="A400" s="1" t="n">
@@ -14379,9 +13180,6 @@
       <c r="J400" t="n">
         <v>55</v>
       </c>
-      <c r="K400" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="401">
       <c r="A401" s="1" t="n">
@@ -14414,9 +13212,6 @@
       <c r="J401" t="n">
         <v>47</v>
       </c>
-      <c r="K401" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="402">
       <c r="A402" s="1" t="n">
@@ -14449,9 +13244,6 @@
       <c r="J402" t="n">
         <v>49</v>
       </c>
-      <c r="K402" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="403">
       <c r="A403" s="1" t="n">
@@ -14484,9 +13276,6 @@
       <c r="J403" t="n">
         <v>49</v>
       </c>
-      <c r="K403" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="404">
       <c r="A404" s="1" t="n">
@@ -14519,9 +13308,6 @@
       <c r="J404" t="n">
         <v>62</v>
       </c>
-      <c r="K404" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="405">
       <c r="A405" s="1" t="n">
@@ -14554,9 +13340,6 @@
       <c r="J405" t="n">
         <v>58</v>
       </c>
-      <c r="K405" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="406">
       <c r="A406" s="1" t="n">
@@ -14589,9 +13372,6 @@
       <c r="J406" t="n">
         <v>57</v>
       </c>
-      <c r="K406" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="407">
       <c r="A407" s="1" t="n">
@@ -14624,9 +13404,6 @@
       <c r="J407" t="n">
         <v>51</v>
       </c>
-      <c r="K407" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="408">
       <c r="A408" s="1" t="n">
@@ -14659,9 +13436,6 @@
       <c r="J408" t="n">
         <v>61</v>
       </c>
-      <c r="K408" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="409">
       <c r="A409" s="1" t="n">
@@ -14694,9 +13468,6 @@
       <c r="J409" t="n">
         <v>60</v>
       </c>
-      <c r="K409" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="410">
       <c r="A410" s="1" t="n">
@@ -14729,9 +13500,6 @@
       <c r="J410" t="n">
         <v>40</v>
       </c>
-      <c r="K410" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="411">
       <c r="A411" s="1" t="n">
@@ -14764,9 +13532,6 @@
       <c r="J411" t="n">
         <v>16</v>
       </c>
-      <c r="K411" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="412">
       <c r="A412" s="1" t="n">
@@ -14799,9 +13564,6 @@
       <c r="J412" t="n">
         <v>62</v>
       </c>
-      <c r="K412" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="413">
       <c r="A413" s="1" t="n">
@@ -14834,9 +13596,6 @@
       <c r="J413" t="n">
         <v>60</v>
       </c>
-      <c r="K413" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="414">
       <c r="A414" s="1" t="n">
@@ -14869,9 +13628,6 @@
       <c r="J414" t="n">
         <v>55</v>
       </c>
-      <c r="K414" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="415">
       <c r="A415" s="1" t="n">
@@ -14904,9 +13660,6 @@
       <c r="J415" t="n">
         <v>63</v>
       </c>
-      <c r="K415" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="416">
       <c r="A416" s="1" t="n">
@@ -14939,9 +13692,6 @@
       <c r="J416" t="n">
         <v>46</v>
       </c>
-      <c r="K416" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="417">
       <c r="A417" s="1" t="n">
@@ -14974,9 +13724,6 @@
       <c r="J417" t="n">
         <v>39</v>
       </c>
-      <c r="K417" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="418">
       <c r="A418" s="1" t="n">
@@ -15009,9 +13756,6 @@
       <c r="J418" t="n">
         <v>60</v>
       </c>
-      <c r="K418" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="419">
       <c r="A419" s="1" t="n">
@@ -15044,9 +13788,6 @@
       <c r="J419" t="n">
         <v>45</v>
       </c>
-      <c r="K419" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="420">
       <c r="A420" s="1" t="n">
@@ -15079,9 +13820,6 @@
       <c r="J420" t="n">
         <v>48</v>
       </c>
-      <c r="K420" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="421">
       <c r="A421" s="1" t="n">
@@ -15114,9 +13852,6 @@
       <c r="J421" t="n">
         <v>41</v>
       </c>
-      <c r="K421" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="422">
       <c r="A422" s="1" t="n">
@@ -15149,9 +13884,6 @@
       <c r="J422" t="n">
         <v>43</v>
       </c>
-      <c r="K422" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="423">
       <c r="A423" s="1" t="n">
@@ -15184,9 +13916,6 @@
       <c r="J423" t="n">
         <v>63</v>
       </c>
-      <c r="K423" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="424">
       <c r="A424" s="1" t="n">
@@ -15219,9 +13948,6 @@
       <c r="J424" t="n">
         <v>55</v>
       </c>
-      <c r="K424" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="425">
       <c r="A425" s="1" t="n">
@@ -15254,9 +13980,6 @@
       <c r="J425" t="n">
         <v>61</v>
       </c>
-      <c r="K425" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="426">
       <c r="A426" s="1" t="n">
@@ -15289,9 +14012,6 @@
       <c r="J426" t="n">
         <v>42</v>
       </c>
-      <c r="K426" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="427">
       <c r="A427" s="1" t="n">
@@ -15324,9 +14044,6 @@
       <c r="J427" t="n">
         <v>33</v>
       </c>
-      <c r="K427" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="428">
       <c r="A428" s="1" t="n">
@@ -15359,9 +14076,6 @@
       <c r="J428" t="n">
         <v>33</v>
       </c>
-      <c r="K428" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="429">
       <c r="A429" s="1" t="n">
@@ -15394,9 +14108,6 @@
       <c r="J429" t="n">
         <v>49</v>
       </c>
-      <c r="K429" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="430">
       <c r="A430" s="1" t="n">
@@ -15429,9 +14140,6 @@
       <c r="J430" t="n">
         <v>34</v>
       </c>
-      <c r="K430" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="431">
       <c r="A431" s="1" t="n">
@@ -15464,9 +14172,6 @@
       <c r="J431" t="n">
         <v>32</v>
       </c>
-      <c r="K431" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="432">
       <c r="A432" s="1" t="n">
@@ -15499,9 +14204,6 @@
       <c r="J432" t="n">
         <v>16</v>
       </c>
-      <c r="K432" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="433">
       <c r="A433" s="1" t="n">
@@ -15534,9 +14236,6 @@
       <c r="J433" t="n">
         <v>16</v>
       </c>
-      <c r="K433" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="434">
       <c r="A434" s="1" t="n">
@@ -15569,9 +14268,6 @@
       <c r="J434" t="n">
         <v>16</v>
       </c>
-      <c r="K434" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="435">
       <c r="A435" s="1" t="n">
@@ -15604,9 +14300,6 @@
       <c r="J435" t="n">
         <v>18</v>
       </c>
-      <c r="K435" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="436">
       <c r="A436" s="1" t="n">
@@ -15639,9 +14332,6 @@
       <c r="J436" t="n">
         <v>16</v>
       </c>
-      <c r="K436" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="437">
       <c r="A437" s="1" t="n">
@@ -15674,9 +14364,6 @@
       <c r="J437" t="n">
         <v>16</v>
       </c>
-      <c r="K437" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="438">
       <c r="A438" s="1" t="n">
@@ -15709,9 +14396,6 @@
       <c r="J438" t="n">
         <v>17</v>
       </c>
-      <c r="K438" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="439">
       <c r="A439" s="1" t="n">
@@ -15744,9 +14428,6 @@
       <c r="J439" t="n">
         <v>16</v>
       </c>
-      <c r="K439" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="440">
       <c r="A440" s="1" t="n">
@@ -15779,9 +14460,6 @@
       <c r="J440" t="n">
         <v>31</v>
       </c>
-      <c r="K440" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="441">
       <c r="A441" s="1" t="n">
@@ -15814,9 +14492,6 @@
       <c r="J441" t="n">
         <v>40</v>
       </c>
-      <c r="K441" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="442">
       <c r="A442" s="1" t="n">
@@ -15849,9 +14524,6 @@
       <c r="J442" t="n">
         <v>32</v>
       </c>
-      <c r="K442" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="443">
       <c r="A443" s="1" t="n">
@@ -15884,9 +14556,6 @@
       <c r="J443" t="n">
         <v>16</v>
       </c>
-      <c r="K443" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="444">
       <c r="A444" s="1" t="n">
@@ -15919,9 +14588,6 @@
       <c r="J444" t="n">
         <v>52</v>
       </c>
-      <c r="K444" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="445">
       <c r="A445" s="1" t="n">
@@ -15954,9 +14620,6 @@
       <c r="J445" t="n">
         <v>37</v>
       </c>
-      <c r="K445" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="446">
       <c r="A446" s="1" t="n">
@@ -15989,9 +14652,6 @@
       <c r="J446" t="n">
         <v>27</v>
       </c>
-      <c r="K446" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="447">
       <c r="A447" s="1" t="n">
@@ -16024,9 +14684,6 @@
       <c r="J447" t="n">
         <v>25</v>
       </c>
-      <c r="K447" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="448">
       <c r="A448" s="1" t="n">
@@ -16059,9 +14716,6 @@
       <c r="J448" t="n">
         <v>34</v>
       </c>
-      <c r="K448" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="449">
       <c r="A449" s="1" t="n">
@@ -16094,9 +14748,6 @@
       <c r="J449" t="n">
         <v>17</v>
       </c>
-      <c r="K449" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="450">
       <c r="A450" s="1" t="n">
@@ -16129,9 +14780,6 @@
       <c r="J450" t="n">
         <v>20</v>
       </c>
-      <c r="K450" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="451">
       <c r="A451" s="1" t="n">
@@ -16164,9 +14812,6 @@
       <c r="J451" t="n">
         <v>48</v>
       </c>
-      <c r="K451" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="452">
       <c r="A452" s="1" t="n">
@@ -16199,9 +14844,6 @@
       <c r="J452" t="n">
         <v>24</v>
       </c>
-      <c r="K452" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="453">
       <c r="A453" s="1" t="n">
@@ -16234,9 +14876,6 @@
       <c r="J453" t="n">
         <v>18</v>
       </c>
-      <c r="K453" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="454">
       <c r="A454" s="1" t="n">
@@ -16269,9 +14908,6 @@
       <c r="J454" t="n">
         <v>42</v>
       </c>
-      <c r="K454" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="455">
       <c r="A455" s="1" t="n">
@@ -16304,9 +14940,6 @@
       <c r="J455" t="n">
         <v>51</v>
       </c>
-      <c r="K455" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="456">
       <c r="A456" s="1" t="n">
@@ -16339,9 +14972,6 @@
       <c r="J456" t="n">
         <v>39</v>
       </c>
-      <c r="K456" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="457">
       <c r="A457" s="1" t="n">
@@ -16374,9 +15004,6 @@
       <c r="J457" t="n">
         <v>27</v>
       </c>
-      <c r="K457" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="458">
       <c r="A458" s="1" t="n">
@@ -16409,9 +15036,6 @@
       <c r="J458" t="n">
         <v>57</v>
       </c>
-      <c r="K458" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="459">
       <c r="A459" s="1" t="n">
@@ -16444,9 +15068,6 @@
       <c r="J459" t="n">
         <v>58</v>
       </c>
-      <c r="K459" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="460">
       <c r="A460" s="1" t="n">
@@ -16479,9 +15100,6 @@
       <c r="J460" t="n">
         <v>52</v>
       </c>
-      <c r="K460" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="461">
       <c r="A461" s="1" t="n">
@@ -16514,9 +15132,6 @@
       <c r="J461" t="n">
         <v>55</v>
       </c>
-      <c r="K461" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="462">
       <c r="A462" s="1" t="n">
@@ -16549,9 +15164,6 @@
       <c r="J462" t="n">
         <v>40</v>
       </c>
-      <c r="K462" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="463">
       <c r="A463" s="1" t="n">
@@ -16583,9 +15195,6 @@
       </c>
       <c r="J463" t="n">
         <v>46</v>
-      </c>
-      <c r="K463" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>